<commit_message>
added intra/inter class ratio
</commit_message>
<xml_diff>
--- a/results/catgories_results.xlsx
+++ b/results/catgories_results.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3340" yWindow="600" windowWidth="28720" windowHeight="18480" tabRatio="500"/>
+    <workbookView xWindow="2620" yWindow="0" windowWidth="28720" windowHeight="18480" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="27">
   <si>
     <t>mission impossible</t>
   </si>
@@ -89,6 +90,18 @@
   <si>
     <t xml:space="preserve"> normalized laplacian, threshold-28, alpha 0.6 </t>
   </si>
+  <si>
+    <t>non normalized laplacian, threshold-28, alpha 1.8141e-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> normalized laplacian, threshold-28, alpha 1.5</t>
+  </si>
+  <si>
+    <t>non normalized laplacian, threshold-28, alpha 4.5354e-04</t>
+  </si>
+  <si>
+    <t>intraclass/interclass ratio</t>
+  </si>
 </sst>
 </file>
 
@@ -149,8 +162,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -169,19 +206,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -190,6 +251,187 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="temp.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10058400" y="495300"/>
+          <a:ext cx="7112000" cy="5334000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="temp.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10045700" y="6692900"/>
+          <a:ext cx="7112000" cy="5334000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="temp.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9906000" y="12661900"/>
+          <a:ext cx="7112000" cy="5334000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="temp2.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9918700" y="18859500"/>
+          <a:ext cx="7112000" cy="5334000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -604,10 +846,1649 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A13:V114"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="48.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="31.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="13" spans="1:22">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" t="s">
+        <v>8</v>
+      </c>
+      <c r="K13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.97892999999999997</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1.0526</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.96374000000000004</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1.0764</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1.0235000000000001</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1.0622</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0.79427000000000003</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1.1427</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1.0962000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.97892999999999997</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1.0528999999999999</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.96240000000000003</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1.0751999999999999</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1.0223</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1.0609999999999999</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0.79481999999999997</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1.1415999999999999</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1.095</v>
+      </c>
+      <c r="V15" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.0526</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1.0528999999999999</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1.0390999999999999</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1.1443000000000001</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1.0948</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1.1309</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0.88622000000000001</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1.2069000000000001</v>
+      </c>
+      <c r="K16" s="1">
+        <v>1.163</v>
+      </c>
+      <c r="V16" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.96374000000000004</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.96240000000000003</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1.0390999999999999</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.0488999999999999</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.99431000000000003</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1.0345</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.76698</v>
+      </c>
+      <c r="J17" s="1">
+        <v>1.1238999999999999</v>
+      </c>
+      <c r="K17" s="1">
+        <v>1.0765</v>
+      </c>
+      <c r="V17" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.0764</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1.0751999999999999</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1.1443000000000001</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1.0488999999999999</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1.1034999999999999</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1.1353</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0.90647999999999995</v>
+      </c>
+      <c r="J18" s="1">
+        <v>1.2218</v>
+      </c>
+      <c r="K18" s="1">
+        <v>1.1783999999999999</v>
+      </c>
+      <c r="V18" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1.0235000000000001</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1.0223</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1.0948</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.99431000000000003</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1.1034999999999999</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1.0898000000000001</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0.84092</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1.1755</v>
+      </c>
+      <c r="K19" s="1">
+        <v>1.1303000000000001</v>
+      </c>
+      <c r="V19" s="2"/>
+    </row>
+    <row r="20" spans="1:22">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1.0622</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1.0609999999999999</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1.1309</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1.0345</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1.1353</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1.0898000000000001</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0.88941999999999999</v>
+      </c>
+      <c r="J20" s="1">
+        <v>1.2093</v>
+      </c>
+      <c r="K20" s="1">
+        <v>1.1654</v>
+      </c>
+      <c r="V20" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.79427000000000003</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.79481999999999997</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.88622000000000001</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.76698</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.90647999999999995</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.84092</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0.88941999999999999</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0.98162000000000005</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0.92745</v>
+      </c>
+      <c r="V21" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1.1427</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1.1415999999999999</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1.2069000000000001</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1.1238999999999999</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1.2218</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1.1755</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1.2093</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0.98162000000000005</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
+        <v>1.2334000000000001</v>
+      </c>
+      <c r="V22" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1.0962000000000001</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1.095</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1.163</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1.0765</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1.1783999999999999</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1.1303000000000001</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1.1654</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0.92745</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1.2334000000000001</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0</v>
+      </c>
+      <c r="V23" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22">
+      <c r="V24" s="2"/>
+    </row>
+    <row r="25" spans="1:22">
+      <c r="V25" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1.0023</v>
+      </c>
+      <c r="V26" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22">
+      <c r="V27" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F39" t="s">
+        <v>4</v>
+      </c>
+      <c r="G39" t="s">
+        <v>5</v>
+      </c>
+      <c r="H39" t="s">
+        <v>6</v>
+      </c>
+      <c r="I39" t="s">
+        <v>7</v>
+      </c>
+      <c r="J39" t="s">
+        <v>8</v>
+      </c>
+      <c r="K39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0.88051999999999997</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0.87736999999999998</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0.88883999999999996</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0.88983999999999996</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0.88895999999999997</v>
+      </c>
+      <c r="H40" s="1">
+        <v>0.88953000000000004</v>
+      </c>
+      <c r="I40" s="1">
+        <v>0.8841</v>
+      </c>
+      <c r="J40" s="1">
+        <v>0.88643000000000005</v>
+      </c>
+      <c r="K40" s="1">
+        <v>0.88656999999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0.88051999999999997</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0.87956999999999996</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0.88878999999999997</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0.88980999999999999</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0.88890999999999998</v>
+      </c>
+      <c r="H41" s="1">
+        <v>0.88949999999999996</v>
+      </c>
+      <c r="I41" s="1">
+        <v>0.8871</v>
+      </c>
+      <c r="J41" s="1">
+        <v>0.88644999999999996</v>
+      </c>
+      <c r="K41" s="1">
+        <v>0.88648000000000005</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0.87736999999999998</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0.87956999999999996</v>
+      </c>
+      <c r="D42" s="1">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0.88870000000000005</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0.88966999999999996</v>
+      </c>
+      <c r="G42" s="1">
+        <v>0.88882000000000005</v>
+      </c>
+      <c r="H42" s="1">
+        <v>0.88936000000000004</v>
+      </c>
+      <c r="I42" s="1">
+        <v>0.88700999999999997</v>
+      </c>
+      <c r="J42" s="1">
+        <v>0.88631000000000004</v>
+      </c>
+      <c r="K42" s="1">
+        <v>0.88639999999999997</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0.88883999999999996</v>
+      </c>
+      <c r="C43" s="1">
+        <v>0.88878999999999997</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0.88870000000000005</v>
+      </c>
+      <c r="E43" s="1">
+        <v>0</v>
+      </c>
+      <c r="F43" s="1">
+        <v>0.87649999999999995</v>
+      </c>
+      <c r="G43" s="1">
+        <v>0.87672000000000005</v>
+      </c>
+      <c r="H43" s="1">
+        <v>0.87709000000000004</v>
+      </c>
+      <c r="I43" s="1">
+        <v>0.88593</v>
+      </c>
+      <c r="J43" s="1">
+        <v>0.88773000000000002</v>
+      </c>
+      <c r="K43" s="1">
+        <v>0.88778999999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0.88983999999999996</v>
+      </c>
+      <c r="C44" s="1">
+        <v>0.88980999999999999</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0.88966999999999996</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0.87649999999999995</v>
+      </c>
+      <c r="F44" s="1">
+        <v>0</v>
+      </c>
+      <c r="G44" s="1">
+        <v>0.87611000000000006</v>
+      </c>
+      <c r="H44" s="1">
+        <v>0.86946000000000001</v>
+      </c>
+      <c r="I44" s="1">
+        <v>0.88958999999999999</v>
+      </c>
+      <c r="J44" s="1">
+        <v>0.88871999999999995</v>
+      </c>
+      <c r="K44" s="1">
+        <v>0.88885000000000003</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0.88895999999999997</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0.88890999999999998</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0.88882000000000005</v>
+      </c>
+      <c r="E45" s="1">
+        <v>0.87672000000000005</v>
+      </c>
+      <c r="F45" s="1">
+        <v>0.87611000000000006</v>
+      </c>
+      <c r="G45" s="1">
+        <v>0</v>
+      </c>
+      <c r="H45" s="1">
+        <v>0.87658999999999998</v>
+      </c>
+      <c r="I45" s="1">
+        <v>0.88560000000000005</v>
+      </c>
+      <c r="J45" s="1">
+        <v>0.88783999999999996</v>
+      </c>
+      <c r="K45" s="1">
+        <v>0.88790999999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.88953000000000004</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0.88949999999999996</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0.88936000000000004</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0.87709000000000004</v>
+      </c>
+      <c r="F46" s="1">
+        <v>0.86946000000000001</v>
+      </c>
+      <c r="G46" s="1">
+        <v>0.87658999999999998</v>
+      </c>
+      <c r="H46" s="1">
+        <v>0</v>
+      </c>
+      <c r="I46" s="1">
+        <v>0.88914000000000004</v>
+      </c>
+      <c r="J46" s="1">
+        <v>0.88839999999999997</v>
+      </c>
+      <c r="K46" s="1">
+        <v>0.88851999999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0.8841</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0.8871</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0.88700999999999997</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0.88593</v>
+      </c>
+      <c r="F47" s="1">
+        <v>0.88958999999999999</v>
+      </c>
+      <c r="G47" s="1">
+        <v>0.88560000000000005</v>
+      </c>
+      <c r="H47" s="1">
+        <v>0.88914000000000004</v>
+      </c>
+      <c r="I47" s="1">
+        <v>0</v>
+      </c>
+      <c r="J47" s="1">
+        <v>0.87621000000000004</v>
+      </c>
+      <c r="K47" s="1">
+        <v>0.88046999999999997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0.88643000000000005</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0.88644999999999996</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0.88631000000000004</v>
+      </c>
+      <c r="E48" s="1">
+        <v>0.88773000000000002</v>
+      </c>
+      <c r="F48" s="1">
+        <v>0.88871999999999995</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0.88783999999999996</v>
+      </c>
+      <c r="H48" s="1">
+        <v>0.88839999999999997</v>
+      </c>
+      <c r="I48" s="1">
+        <v>0.87621000000000004</v>
+      </c>
+      <c r="J48" s="1">
+        <v>0</v>
+      </c>
+      <c r="K48" s="1">
+        <v>0.87175000000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" s="1">
+        <v>0.88656999999999997</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0.88648000000000005</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0.88639999999999997</v>
+      </c>
+      <c r="E49" s="1">
+        <v>0.88778999999999997</v>
+      </c>
+      <c r="F49" s="1">
+        <v>0.88885000000000003</v>
+      </c>
+      <c r="G49" s="1">
+        <v>0.88790999999999998</v>
+      </c>
+      <c r="H49" s="1">
+        <v>0.88851999999999998</v>
+      </c>
+      <c r="I49" s="1">
+        <v>0.88046999999999997</v>
+      </c>
+      <c r="J49" s="1">
+        <v>0.87175000000000002</v>
+      </c>
+      <c r="K49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53">
+        <v>0.98709999999999998</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" t="s">
+        <v>25</v>
+      </c>
+      <c r="B71" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1</v>
+      </c>
+      <c r="D71" t="s">
+        <v>2</v>
+      </c>
+      <c r="E71" t="s">
+        <v>3</v>
+      </c>
+      <c r="F71" t="s">
+        <v>4</v>
+      </c>
+      <c r="G71" t="s">
+        <v>5</v>
+      </c>
+      <c r="H71" t="s">
+        <v>6</v>
+      </c>
+      <c r="I71" t="s">
+        <v>7</v>
+      </c>
+      <c r="J71" t="s">
+        <v>8</v>
+      </c>
+      <c r="K71" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" s="1">
+        <v>0</v>
+      </c>
+      <c r="C72" s="1">
+        <v>0.67025000000000001</v>
+      </c>
+      <c r="D72" s="1">
+        <v>0.76885999999999999</v>
+      </c>
+      <c r="E72" s="1">
+        <v>0.65547</v>
+      </c>
+      <c r="F72" s="1">
+        <v>0.80769999999999997</v>
+      </c>
+      <c r="G72" s="1">
+        <v>0.72848000000000002</v>
+      </c>
+      <c r="H72" s="1">
+        <v>0.78485000000000005</v>
+      </c>
+      <c r="I72" s="1">
+        <v>0.51939999999999997</v>
+      </c>
+      <c r="J72" s="1">
+        <v>0.92798999999999998</v>
+      </c>
+      <c r="K72" s="1">
+        <v>0.83950000000000002</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73" t="s">
+        <v>1</v>
+      </c>
+      <c r="B73" s="1">
+        <v>0.67025000000000001</v>
+      </c>
+      <c r="C73" s="1">
+        <v>0</v>
+      </c>
+      <c r="D73" s="1">
+        <v>0.76976999999999995</v>
+      </c>
+      <c r="E73" s="1">
+        <v>0.65388999999999997</v>
+      </c>
+      <c r="F73" s="1">
+        <v>0.80640999999999996</v>
+      </c>
+      <c r="G73" s="1">
+        <v>0.72702999999999995</v>
+      </c>
+      <c r="H73" s="1">
+        <v>0.78352999999999995</v>
+      </c>
+      <c r="I73" s="1">
+        <v>0.51954999999999996</v>
+      </c>
+      <c r="J73" s="1">
+        <v>0.92696000000000001</v>
+      </c>
+      <c r="K73" s="1">
+        <v>0.83816000000000002</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
+      <c r="A74" t="s">
+        <v>2</v>
+      </c>
+      <c r="B74" s="1">
+        <v>0.76885999999999999</v>
+      </c>
+      <c r="C74" s="1">
+        <v>0.76976999999999995</v>
+      </c>
+      <c r="D74" s="1">
+        <v>0</v>
+      </c>
+      <c r="E74" s="1">
+        <v>0.75844999999999996</v>
+      </c>
+      <c r="F74" s="1">
+        <v>0.89317000000000002</v>
+      </c>
+      <c r="G74" s="1">
+        <v>0.82233000000000001</v>
+      </c>
+      <c r="H74" s="1">
+        <v>0.87258999999999998</v>
+      </c>
+      <c r="I74" s="1">
+        <v>0.64627000000000001</v>
+      </c>
+      <c r="J74" s="1">
+        <v>1.0034000000000001</v>
+      </c>
+      <c r="K74" s="1">
+        <v>0.92206999999999995</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="A75" t="s">
+        <v>3</v>
+      </c>
+      <c r="B75" s="1">
+        <v>0.65547</v>
+      </c>
+      <c r="C75" s="1">
+        <v>0.65388999999999997</v>
+      </c>
+      <c r="D75" s="1">
+        <v>0.75844999999999996</v>
+      </c>
+      <c r="E75" s="1">
+        <v>0</v>
+      </c>
+      <c r="F75" s="1">
+        <v>0.77453000000000005</v>
+      </c>
+      <c r="G75" s="1">
+        <v>0.69281999999999999</v>
+      </c>
+      <c r="H75" s="1">
+        <v>0.75143000000000004</v>
+      </c>
+      <c r="I75" s="1">
+        <v>0.48687000000000002</v>
+      </c>
+      <c r="J75" s="1">
+        <v>0.91</v>
+      </c>
+      <c r="K75" s="1">
+        <v>0.81940000000000002</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76" t="s">
+        <v>4</v>
+      </c>
+      <c r="B76" s="1">
+        <v>0.80769999999999997</v>
+      </c>
+      <c r="C76" s="1">
+        <v>0.80640999999999996</v>
+      </c>
+      <c r="D76" s="1">
+        <v>0.89317000000000002</v>
+      </c>
+      <c r="E76" s="1">
+        <v>0.77453000000000005</v>
+      </c>
+      <c r="F76" s="1">
+        <v>0</v>
+      </c>
+      <c r="G76" s="1">
+        <v>0.83469000000000004</v>
+      </c>
+      <c r="H76" s="1">
+        <v>0.87651000000000001</v>
+      </c>
+      <c r="I76" s="1">
+        <v>0.67964999999999998</v>
+      </c>
+      <c r="J76" s="1">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="K76" s="1">
+        <v>0.94564999999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="A77" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77" s="1">
+        <v>0.72848000000000002</v>
+      </c>
+      <c r="C77" s="1">
+        <v>0.72702999999999995</v>
+      </c>
+      <c r="D77" s="1">
+        <v>0.82233000000000001</v>
+      </c>
+      <c r="E77" s="1">
+        <v>0.69281999999999999</v>
+      </c>
+      <c r="F77" s="1">
+        <v>0.83469000000000004</v>
+      </c>
+      <c r="G77" s="1">
+        <v>0</v>
+      </c>
+      <c r="H77" s="1">
+        <v>0.81347000000000003</v>
+      </c>
+      <c r="I77" s="1">
+        <v>0.58137000000000005</v>
+      </c>
+      <c r="J77" s="1">
+        <v>0.96384999999999998</v>
+      </c>
+      <c r="K77" s="1">
+        <v>0.87885999999999997</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="A78" t="s">
+        <v>6</v>
+      </c>
+      <c r="B78" s="1">
+        <v>0.78485000000000005</v>
+      </c>
+      <c r="C78" s="1">
+        <v>0.78352999999999995</v>
+      </c>
+      <c r="D78" s="1">
+        <v>0.87258999999999998</v>
+      </c>
+      <c r="E78" s="1">
+        <v>0.75143000000000004</v>
+      </c>
+      <c r="F78" s="1">
+        <v>0.87651000000000001</v>
+      </c>
+      <c r="G78" s="1">
+        <v>0.81347000000000003</v>
+      </c>
+      <c r="H78" s="1">
+        <v>0</v>
+      </c>
+      <c r="I78" s="1">
+        <v>0.65215000000000001</v>
+      </c>
+      <c r="J78" s="1">
+        <v>1.0071000000000001</v>
+      </c>
+      <c r="K78" s="1">
+        <v>0.92618</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
+      <c r="A79" t="s">
+        <v>7</v>
+      </c>
+      <c r="B79" s="1">
+        <v>0.51939999999999997</v>
+      </c>
+      <c r="C79" s="1">
+        <v>0.51954999999999996</v>
+      </c>
+      <c r="D79" s="1">
+        <v>0.64627000000000001</v>
+      </c>
+      <c r="E79" s="1">
+        <v>0.48687000000000002</v>
+      </c>
+      <c r="F79" s="1">
+        <v>0.67964999999999998</v>
+      </c>
+      <c r="G79" s="1">
+        <v>0.58137000000000005</v>
+      </c>
+      <c r="H79" s="1">
+        <v>0.65215000000000001</v>
+      </c>
+      <c r="I79" s="1">
+        <v>0</v>
+      </c>
+      <c r="J79" s="1">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="K79" s="1">
+        <v>0.71453</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
+      <c r="A80" t="s">
+        <v>8</v>
+      </c>
+      <c r="B80" s="1">
+        <v>0.92798999999999998</v>
+      </c>
+      <c r="C80" s="1">
+        <v>0.92696000000000001</v>
+      </c>
+      <c r="D80" s="1">
+        <v>1.0034000000000001</v>
+      </c>
+      <c r="E80" s="1">
+        <v>0.91</v>
+      </c>
+      <c r="F80" s="1">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="G80" s="1">
+        <v>0.96384999999999998</v>
+      </c>
+      <c r="H80" s="1">
+        <v>1.0071000000000001</v>
+      </c>
+      <c r="I80" s="1">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="J80" s="1">
+        <v>0</v>
+      </c>
+      <c r="K80" s="1">
+        <v>1.0394000000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11">
+      <c r="A81" t="s">
+        <v>9</v>
+      </c>
+      <c r="B81" s="1">
+        <v>0.83950000000000002</v>
+      </c>
+      <c r="C81" s="1">
+        <v>0.83816000000000002</v>
+      </c>
+      <c r="D81" s="1">
+        <v>0.92206999999999995</v>
+      </c>
+      <c r="E81" s="1">
+        <v>0.81940000000000002</v>
+      </c>
+      <c r="F81" s="1">
+        <v>0.94564999999999999</v>
+      </c>
+      <c r="G81" s="1">
+        <v>0.87885999999999997</v>
+      </c>
+      <c r="H81" s="1">
+        <v>0.92618</v>
+      </c>
+      <c r="I81" s="1">
+        <v>0.71453</v>
+      </c>
+      <c r="J81" s="1">
+        <v>1.0394000000000001</v>
+      </c>
+      <c r="K81" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11">
+      <c r="A85" t="s">
+        <v>26</v>
+      </c>
+      <c r="B85">
+        <v>0.99519999999999997</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11">
+      <c r="A101" t="s">
+        <v>24</v>
+      </c>
+      <c r="B101" t="s">
+        <v>0</v>
+      </c>
+      <c r="C101" t="s">
+        <v>1</v>
+      </c>
+      <c r="D101" t="s">
+        <v>2</v>
+      </c>
+      <c r="E101" t="s">
+        <v>3</v>
+      </c>
+      <c r="F101" t="s">
+        <v>4</v>
+      </c>
+      <c r="G101" t="s">
+        <v>5</v>
+      </c>
+      <c r="H101" t="s">
+        <v>6</v>
+      </c>
+      <c r="I101" t="s">
+        <v>7</v>
+      </c>
+      <c r="J101" t="s">
+        <v>8</v>
+      </c>
+      <c r="K101" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11">
+      <c r="A102" t="s">
+        <v>0</v>
+      </c>
+      <c r="B102" s="1">
+        <v>0</v>
+      </c>
+      <c r="C102" s="1">
+        <v>0.56303999999999998</v>
+      </c>
+      <c r="D102" s="1">
+        <v>0.55952000000000002</v>
+      </c>
+      <c r="E102" s="1">
+        <v>0.57672999999999996</v>
+      </c>
+      <c r="F102" s="1">
+        <v>0.57874000000000003</v>
+      </c>
+      <c r="G102" s="1">
+        <v>0.57682</v>
+      </c>
+      <c r="H102" s="1">
+        <v>0.57808999999999999</v>
+      </c>
+      <c r="I102" s="1">
+        <v>0.56950999999999996</v>
+      </c>
+      <c r="J102" s="1">
+        <v>0.57086000000000003</v>
+      </c>
+      <c r="K102" s="1">
+        <v>0.57106000000000001</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11">
+      <c r="A103" t="s">
+        <v>1</v>
+      </c>
+      <c r="B103" s="1">
+        <v>0.56303999999999998</v>
+      </c>
+      <c r="C103" s="1">
+        <v>0</v>
+      </c>
+      <c r="D103" s="1">
+        <v>0.56205000000000005</v>
+      </c>
+      <c r="E103" s="1">
+        <v>0.57659000000000005</v>
+      </c>
+      <c r="F103" s="1">
+        <v>0.57867000000000002</v>
+      </c>
+      <c r="G103" s="1">
+        <v>0.57669000000000004</v>
+      </c>
+      <c r="H103" s="1">
+        <v>0.57803000000000004</v>
+      </c>
+      <c r="I103" s="1">
+        <v>0.57306999999999997</v>
+      </c>
+      <c r="J103" s="1">
+        <v>0.57094999999999996</v>
+      </c>
+      <c r="K103" s="1">
+        <v>0.57093000000000005</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11">
+      <c r="A104" t="s">
+        <v>2</v>
+      </c>
+      <c r="B104" s="1">
+        <v>0.55952000000000002</v>
+      </c>
+      <c r="C104" s="1">
+        <v>0.56205000000000005</v>
+      </c>
+      <c r="D104" s="1">
+        <v>0</v>
+      </c>
+      <c r="E104" s="1">
+        <v>0.57626999999999995</v>
+      </c>
+      <c r="F104" s="1">
+        <v>0.57811000000000001</v>
+      </c>
+      <c r="G104" s="1">
+        <v>0.57630000000000003</v>
+      </c>
+      <c r="H104" s="1">
+        <v>0.57747000000000004</v>
+      </c>
+      <c r="I104" s="1">
+        <v>0.57299</v>
+      </c>
+      <c r="J104" s="1">
+        <v>0.57030000000000003</v>
+      </c>
+      <c r="K104" s="1">
+        <v>0.57042000000000004</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11">
+      <c r="A105" t="s">
+        <v>3</v>
+      </c>
+      <c r="B105" s="1">
+        <v>0.57672999999999996</v>
+      </c>
+      <c r="C105" s="1">
+        <v>0.57659000000000005</v>
+      </c>
+      <c r="D105" s="1">
+        <v>0.57626999999999995</v>
+      </c>
+      <c r="E105" s="1">
+        <v>0</v>
+      </c>
+      <c r="F105" s="1">
+        <v>0.55879999999999996</v>
+      </c>
+      <c r="G105" s="1">
+        <v>0.55850999999999995</v>
+      </c>
+      <c r="H105" s="1">
+        <v>0.55930999999999997</v>
+      </c>
+      <c r="I105" s="1">
+        <v>0.57357999999999998</v>
+      </c>
+      <c r="J105" s="1">
+        <v>0.57428999999999997</v>
+      </c>
+      <c r="K105" s="1">
+        <v>0.57432000000000005</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11">
+      <c r="A106" t="s">
+        <v>4</v>
+      </c>
+      <c r="B106" s="1">
+        <v>0.57874000000000003</v>
+      </c>
+      <c r="C106" s="1">
+        <v>0.57867000000000002</v>
+      </c>
+      <c r="D106" s="1">
+        <v>0.57811000000000001</v>
+      </c>
+      <c r="E106" s="1">
+        <v>0.55879999999999996</v>
+      </c>
+      <c r="F106" s="1">
+        <v>0</v>
+      </c>
+      <c r="G106" s="1">
+        <v>0.55833999999999995</v>
+      </c>
+      <c r="H106" s="1">
+        <v>0.55122000000000004</v>
+      </c>
+      <c r="I106" s="1">
+        <v>0.57908000000000004</v>
+      </c>
+      <c r="J106" s="1">
+        <v>0.57606000000000002</v>
+      </c>
+      <c r="K106" s="1">
+        <v>0.57626999999999995</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11">
+      <c r="A107" t="s">
+        <v>5</v>
+      </c>
+      <c r="B107" s="1">
+        <v>0.57682</v>
+      </c>
+      <c r="C107" s="1">
+        <v>0.57669000000000004</v>
+      </c>
+      <c r="D107" s="1">
+        <v>0.57630000000000003</v>
+      </c>
+      <c r="E107" s="1">
+        <v>0.55850999999999995</v>
+      </c>
+      <c r="F107" s="1">
+        <v>0.55833999999999995</v>
+      </c>
+      <c r="G107" s="1">
+        <v>0</v>
+      </c>
+      <c r="H107" s="1">
+        <v>0.55879999999999996</v>
+      </c>
+      <c r="I107" s="1">
+        <v>0.57376000000000005</v>
+      </c>
+      <c r="J107" s="1">
+        <v>0.57425999999999999</v>
+      </c>
+      <c r="K107" s="1">
+        <v>0.57433999999999996</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11">
+      <c r="A108" t="s">
+        <v>6</v>
+      </c>
+      <c r="B108" s="1">
+        <v>0.57808999999999999</v>
+      </c>
+      <c r="C108" s="1">
+        <v>0.57803000000000004</v>
+      </c>
+      <c r="D108" s="1">
+        <v>0.57747000000000004</v>
+      </c>
+      <c r="E108" s="1">
+        <v>0.55930999999999997</v>
+      </c>
+      <c r="F108" s="1">
+        <v>0.55122000000000004</v>
+      </c>
+      <c r="G108" s="1">
+        <v>0.55879999999999996</v>
+      </c>
+      <c r="H108" s="1">
+        <v>0</v>
+      </c>
+      <c r="I108" s="1">
+        <v>0.57813999999999999</v>
+      </c>
+      <c r="J108" s="1">
+        <v>0.57543</v>
+      </c>
+      <c r="K108" s="1">
+        <v>0.57560999999999996</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11">
+      <c r="A109" t="s">
+        <v>7</v>
+      </c>
+      <c r="B109" s="1">
+        <v>0.56950999999999996</v>
+      </c>
+      <c r="C109" s="1">
+        <v>0.57306999999999997</v>
+      </c>
+      <c r="D109" s="1">
+        <v>0.57299</v>
+      </c>
+      <c r="E109" s="1">
+        <v>0.57357999999999998</v>
+      </c>
+      <c r="F109" s="1">
+        <v>0.57908000000000004</v>
+      </c>
+      <c r="G109" s="1">
+        <v>0.57376000000000005</v>
+      </c>
+      <c r="H109" s="1">
+        <v>0.57813999999999999</v>
+      </c>
+      <c r="I109" s="1">
+        <v>0</v>
+      </c>
+      <c r="J109" s="1">
+        <v>0.56103000000000003</v>
+      </c>
+      <c r="K109" s="1">
+        <v>0.56545999999999996</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11">
+      <c r="A110" t="s">
+        <v>8</v>
+      </c>
+      <c r="B110" s="1">
+        <v>0.57086000000000003</v>
+      </c>
+      <c r="C110" s="1">
+        <v>0.57094999999999996</v>
+      </c>
+      <c r="D110" s="1">
+        <v>0.57030000000000003</v>
+      </c>
+      <c r="E110" s="1">
+        <v>0.57428999999999997</v>
+      </c>
+      <c r="F110" s="1">
+        <v>0.57606000000000002</v>
+      </c>
+      <c r="G110" s="1">
+        <v>0.57425999999999999</v>
+      </c>
+      <c r="H110" s="1">
+        <v>0.57543</v>
+      </c>
+      <c r="I110" s="1">
+        <v>0.56103000000000003</v>
+      </c>
+      <c r="J110" s="1">
+        <v>0</v>
+      </c>
+      <c r="K110" s="1">
+        <v>0.55388000000000004</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11">
+      <c r="A111" t="s">
+        <v>9</v>
+      </c>
+      <c r="B111" s="1">
+        <v>0.57106000000000001</v>
+      </c>
+      <c r="C111" s="1">
+        <v>0.57093000000000005</v>
+      </c>
+      <c r="D111" s="1">
+        <v>0.57042000000000004</v>
+      </c>
+      <c r="E111" s="1">
+        <v>0.57432000000000005</v>
+      </c>
+      <c r="F111" s="1">
+        <v>0.57626999999999995</v>
+      </c>
+      <c r="G111" s="1">
+        <v>0.57433999999999996</v>
+      </c>
+      <c r="H111" s="1">
+        <v>0.57560999999999996</v>
+      </c>
+      <c r="I111" s="1">
+        <v>0.56545999999999996</v>
+      </c>
+      <c r="J111" s="1">
+        <v>0.55388000000000004</v>
+      </c>
+      <c r="K111" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>26</v>
+      </c>
+      <c r="B114" s="1">
+        <v>0.97250000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X48"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B24" workbookViewId="0">
-      <selection activeCell="L53" sqref="L53"/>
+    <sheetView showRuler="0" topLeftCell="Q2" workbookViewId="0">
+      <selection activeCell="X18" sqref="X18:X30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>